<commit_message>
Big modifications: first real version of the event & impact data output, using IFRC EA data. Next step is adding some hazard data! Need to be careful about how many different variables were modified or deleted.
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/Desinventar_HIP.xlsx
+++ b/Taxonomies/MostlyImpactData/Desinventar_HIP.xlsx
@@ -61,10 +61,10 @@
     <t xml:space="preserve">hazgeoseis</t>
   </si>
   <si>
-    <t xml:space="preserve">GH0001,GH0002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GH0003,GH0004,GH0005,GH0006,GH0007</t>
+    <t xml:space="preserve">GH0001:GH0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GH0003:GH0004:GH0005:GH0006:GH0007</t>
   </si>
   <si>
     <t xml:space="preserve">fire</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">SS</t>
   </si>
   <si>
-    <t xml:space="preserve">hazhmmarine,hazhmflood,hazhmwind</t>
+    <t xml:space="preserve">hazhmmarine:hazhmflood:hazhmwind</t>
   </si>
   <si>
     <t xml:space="preserve">panic</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">DR</t>
   </si>
   <si>
-    <t xml:space="preserve">hazhmprecip,hazhmtemp</t>
+    <t xml:space="preserve">hazhmprecip:hazhmtemp</t>
   </si>
   <si>
     <t xml:space="preserve">tsunami</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">TS</t>
   </si>
   <si>
-    <t xml:space="preserve">hazgeoother,hazhmmarine,hazhmflood</t>
+    <t xml:space="preserve">hazgeoother:hazhmmarine:hazhmflood</t>
   </si>
   <si>
     <t xml:space="preserve">cyclone</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">TC</t>
   </si>
   <si>
-    <t xml:space="preserve">hazhmwind,hazhmpress,hazhmconv,hazhmflood</t>
+    <t xml:space="preserve">hazhmwind:hazhmpress:hazhmconv:hazhmflood</t>
   </si>
   <si>
     <t xml:space="preserve">strong wind</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">VW</t>
   </si>
   <si>
-    <t xml:space="preserve">hazhmwind,hazhmpress</t>
+    <t xml:space="preserve">hazhmwind:hazhmpress</t>
   </si>
   <si>
     <t xml:space="preserve">hailstorm</t>
@@ -184,7 +184,7 @@
     <t xml:space="preserve">tidal wave</t>
   </si>
   <si>
-    <t xml:space="preserve">hazhmmarine,hazhmflood</t>
+    <t xml:space="preserve">hazhmmarine:hazhmflood</t>
   </si>
   <si>
     <t xml:space="preserve">other</t>
@@ -223,7 +223,7 @@
     <t xml:space="preserve">LS</t>
   </si>
   <si>
-    <t xml:space="preserve">hazgeoseis,hazenvenvdeg,hazgeovolc,hazgeoother</t>
+    <t xml:space="preserve">hazgeoseis:hazenvenvdeg:hazgeovolc:hazgeoother</t>
   </si>
   <si>
     <t xml:space="preserve">heat wave</t>
@@ -235,7 +235,7 @@
     <t xml:space="preserve">storm</t>
   </si>
   <si>
-    <t xml:space="preserve">hazhmconv,hazhmwind,hazhmpress,hazhmflood</t>
+    <t xml:space="preserve">hazhmconv:hazhmwind:hazhmpress:hazhmflood</t>
   </si>
   <si>
     <t xml:space="preserve">forest fire</t>
@@ -256,7 +256,7 @@
     <t xml:space="preserve">liquefaction</t>
   </si>
   <si>
-    <t xml:space="preserve">hazgeoseis,hazgeoother</t>
+    <t xml:space="preserve">hazgeoseis:hazgeoother</t>
   </si>
   <si>
     <t xml:space="preserve">leak</t>
@@ -835,7 +835,7 @@
     <t xml:space="preserve">coastal flood</t>
   </si>
   <si>
-    <t xml:space="preserve">hazhmflood,hazhmmarine</t>
+    <t xml:space="preserve">hazhmflood:hazhmmarine</t>
   </si>
   <si>
     <t xml:space="preserve">flooding</t>
@@ -964,7 +964,34 @@
     <t xml:space="preserve">ສັດຕູພືດ</t>
   </si>
   <si>
-    <t xml:space="preserve">ອຸປະຕິເຫດຖ/ໜ</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lohit Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ອຸປະຕິເຫດຖ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lohit Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ໜ</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ຝົນຕົກ</t>
@@ -2113,7 +2140,34 @@
     <t xml:space="preserve">امواج عالية</t>
   </si>
   <si>
-    <t xml:space="preserve">وفاة/اصابة</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lohit Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">وفاة</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lohit Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">اصابة</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">death/injury</t>
@@ -2134,7 +2188,34 @@
     <t xml:space="preserve">انهيار صخور</t>
   </si>
   <si>
-    <t xml:space="preserve">وفاة/مصاب</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lohit Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">وفاة</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lohit Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">مصاب</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">تسونامي</t>
@@ -2168,7 +2249,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2190,6 +2271,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lohit Devanagari"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -2256,7 +2343,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2264,7 +2351,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2274,12 +2361,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2345,22 +2432,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H496"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="87" sqref="F8 F10:F13 F18 F22 F25:F27 F33 F38 F42 F44 F61 F63 F65 F70 F75 F82 F88 F94 F100 F105 F107 F116 F119 F122 F140 F147:F149 F156 F162 F172 F176 F179 F181 F196:F197 F208 F213 F217 F220 F222 F243 F258 F261 F277 F281 F286 F290 F293:F294 F302 F311:F312 F330:F331 F333 F336 F339 F345 F347 F352 F361 F368 F370:F371 F376 F382 F386 F389 F394 F407 F409 F414:F416 F428 F431 F437 F452 F458:F459 F461 F465 F468 F470 F473:F475 F477:F478 F485 F491 G2:H2 G20:H20 G52:H52 G174:H174 G262:H262 G300:H300 G338:H338 G395:H395 G420:H420 H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="10.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5007,7 +5093,7 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="s">
+      <c r="A166" s="2" t="s">
         <v>276</v>
       </c>
       <c r="B166" s="1" t="s">
@@ -5027,7 +5113,7 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="s">
+      <c r="A167" s="2" t="s">
         <v>278</v>
       </c>
       <c r="B167" s="1" t="s">
@@ -5038,7 +5124,7 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="s">
+      <c r="A168" s="2" t="s">
         <v>279</v>
       </c>
       <c r="B168" s="1" t="s">
@@ -5058,7 +5144,7 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="s">
+      <c r="A169" s="2" t="s">
         <v>280</v>
       </c>
       <c r="B169" s="1" t="s">
@@ -5078,7 +5164,7 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1" t="s">
+      <c r="A170" s="2" t="s">
         <v>282</v>
       </c>
       <c r="B170" s="1" t="s">
@@ -5098,7 +5184,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="s">
+      <c r="A171" s="2" t="s">
         <v>283</v>
       </c>
       <c r="B171" s="1" t="s">
@@ -5109,7 +5195,7 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="1" t="s">
+      <c r="A172" s="2" t="s">
         <v>285</v>
       </c>
       <c r="B172" s="1" t="s">
@@ -5129,7 +5215,7 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="1" t="s">
+      <c r="A173" s="2" t="s">
         <v>286</v>
       </c>
       <c r="B173" s="1" t="s">
@@ -5140,7 +5226,7 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="1" t="s">
+      <c r="A174" s="2" t="s">
         <v>287</v>
       </c>
       <c r="B174" s="1" t="s">
@@ -5166,7 +5252,7 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="s">
+      <c r="A175" s="2" t="s">
         <v>288</v>
       </c>
       <c r="B175" s="1" t="s">
@@ -5186,7 +5272,7 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="s">
+      <c r="A176" s="2" t="s">
         <v>289</v>
       </c>
       <c r="B176" s="1" t="s">
@@ -5206,7 +5292,7 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="s">
+      <c r="A177" s="2" t="s">
         <v>290</v>
       </c>
       <c r="B177" s="1" t="s">
@@ -5226,7 +5312,7 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="s">
+      <c r="A178" s="2" t="s">
         <v>291</v>
       </c>
       <c r="B178" s="1" t="s">
@@ -5243,7 +5329,7 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="s">
+      <c r="A179" s="2" t="s">
         <v>292</v>
       </c>
       <c r="B179" s="1" t="s">
@@ -5263,7 +5349,7 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="s">
+      <c r="A180" s="2" t="s">
         <v>293</v>
       </c>
       <c r="B180" s="1" t="s">
@@ -5283,7 +5369,7 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="s">
+      <c r="A181" s="2" t="s">
         <v>294</v>
       </c>
       <c r="B181" s="1" t="s">
@@ -5303,7 +5389,7 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="1" t="s">
+      <c r="A182" s="2" t="s">
         <v>295</v>
       </c>
       <c r="B182" s="1" t="s">
@@ -5323,7 +5409,7 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="1" t="s">
+      <c r="A183" s="2" t="s">
         <v>296</v>
       </c>
       <c r="B183" s="1" t="s">
@@ -5334,7 +5420,7 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="s">
+      <c r="A184" s="2" t="s">
         <v>298</v>
       </c>
       <c r="B184" s="1" t="s">
@@ -5456,7 +5542,7 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="1" t="s">
+      <c r="A194" s="2" t="s">
         <v>308</v>
       </c>
       <c r="B194" s="1" t="s">
@@ -5476,7 +5562,7 @@
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="1" t="s">
+      <c r="A195" s="2" t="s">
         <v>310</v>
       </c>
       <c r="B195" s="1" t="s">
@@ -5516,7 +5602,7 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="1" t="s">
+      <c r="A197" s="2" t="s">
         <v>311</v>
       </c>
       <c r="B197" s="1" t="s">
@@ -5536,7 +5622,7 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="1" t="s">
+      <c r="A198" s="2" t="s">
         <v>312</v>
       </c>
       <c r="B198" s="1" t="s">
@@ -5567,7 +5653,7 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="1" t="s">
+      <c r="A200" s="2" t="s">
         <v>313</v>
       </c>
       <c r="B200" s="1" t="s">
@@ -5578,7 +5664,7 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="1" t="s">
+      <c r="A201" s="2" t="s">
         <v>314</v>
       </c>
       <c r="B201" s="1" t="s">
@@ -5589,7 +5675,7 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="1" t="s">
+      <c r="A202" s="2" t="s">
         <v>315</v>
       </c>
       <c r="B202" s="1" t="s">
@@ -5609,7 +5695,7 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="1" t="s">
+      <c r="A203" s="2" t="s">
         <v>316</v>
       </c>
       <c r="B203" s="1" t="s">
@@ -5626,7 +5712,7 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="1" t="s">
+      <c r="A204" s="2" t="s">
         <v>317</v>
       </c>
       <c r="B204" s="1" t="s">
@@ -5637,7 +5723,7 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="1" t="s">
+      <c r="A205" s="2" t="s">
         <v>319</v>
       </c>
       <c r="B205" s="1" t="s">
@@ -5657,7 +5743,7 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="1" t="s">
+      <c r="A206" s="2" t="s">
         <v>320</v>
       </c>
       <c r="B206" s="1" t="s">
@@ -5668,7 +5754,7 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="1" t="s">
+      <c r="A207" s="2" t="s">
         <v>322</v>
       </c>
       <c r="B207" s="1" t="s">
@@ -6426,10 +6512,10 @@
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="2" t="s">
+      <c r="A259" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="B259" s="2" t="s">
+      <c r="B259" s="3" t="s">
         <v>382</v>
       </c>
       <c r="C259" s="1" t="s">
@@ -6437,10 +6523,10 @@
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="2" t="s">
+      <c r="A260" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="B260" s="2" t="s">
+      <c r="B260" s="3" t="s">
         <v>384</v>
       </c>
       <c r="C260" s="1" t="s">
@@ -6448,10 +6534,10 @@
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="2" t="s">
+      <c r="A261" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="B261" s="2" t="s">
+      <c r="B261" s="3" t="s">
         <v>385</v>
       </c>
       <c r="C261" s="1" t="s">
@@ -6468,7 +6554,7 @@
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="2" t="s">
+      <c r="A262" s="3" t="s">
         <v>386</v>
       </c>
       <c r="B262" s="1" t="s">
@@ -6494,7 +6580,7 @@
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="2" t="s">
+      <c r="A263" s="3" t="s">
         <v>388</v>
       </c>
       <c r="B263" s="3" t="s">
@@ -6517,7 +6603,7 @@
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="2" t="s">
+      <c r="A264" s="3" t="s">
         <v>392</v>
       </c>
       <c r="B264" s="1" t="s">
@@ -6528,7 +6614,7 @@
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="2" t="s">
+      <c r="A265" s="3" t="s">
         <v>394</v>
       </c>
       <c r="B265" s="5" t="s">
@@ -6539,7 +6625,7 @@
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="2" t="s">
+      <c r="A266" s="3" t="s">
         <v>396</v>
       </c>
       <c r="B266" s="5" t="s">
@@ -6550,7 +6636,7 @@
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="2" t="s">
+      <c r="A267" s="3" t="s">
         <v>398</v>
       </c>
       <c r="B267" s="5" t="s">
@@ -6561,7 +6647,7 @@
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="2" t="s">
+      <c r="A268" s="3" t="s">
         <v>400</v>
       </c>
       <c r="B268" s="1" t="s">
@@ -6572,10 +6658,10 @@
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="2" t="s">
+      <c r="A269" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="B269" s="2" t="s">
+      <c r="B269" s="3" t="s">
         <v>403</v>
       </c>
       <c r="C269" s="1" t="s">
@@ -6592,7 +6678,7 @@
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="2" t="s">
+      <c r="A270" s="3" t="s">
         <v>404</v>
       </c>
       <c r="B270" s="1" t="s">
@@ -6603,7 +6689,7 @@
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="2" t="s">
+      <c r="A271" s="3" t="s">
         <v>405</v>
       </c>
       <c r="B271" s="1" t="s">
@@ -6614,7 +6700,7 @@
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="2" t="s">
+      <c r="A272" s="3" t="s">
         <v>406</v>
       </c>
       <c r="B272" s="1" t="s">
@@ -6625,7 +6711,7 @@
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="2" t="s">
+      <c r="A273" s="3" t="s">
         <v>408</v>
       </c>
       <c r="B273" s="1" t="s">
@@ -6636,7 +6722,7 @@
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="2" t="s">
+      <c r="A274" s="3" t="s">
         <v>410</v>
       </c>
       <c r="B274" s="1" t="s">
@@ -6656,7 +6742,7 @@
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="2" t="s">
+      <c r="A275" s="3" t="s">
         <v>411</v>
       </c>
       <c r="B275" s="1" t="s">
@@ -6667,7 +6753,7 @@
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="2" t="s">
+      <c r="A276" s="3" t="s">
         <v>413</v>
       </c>
       <c r="B276" s="1" t="s">
@@ -6678,7 +6764,7 @@
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="2" t="s">
+      <c r="A277" s="3" t="s">
         <v>415</v>
       </c>
       <c r="B277" s="1" t="s">
@@ -6698,7 +6784,7 @@
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="2" t="s">
+      <c r="A278" s="3" t="s">
         <v>416</v>
       </c>
       <c r="B278" s="1" t="s">
@@ -6718,7 +6804,7 @@
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="2" t="s">
+      <c r="A279" s="3" t="s">
         <v>417</v>
       </c>
       <c r="B279" s="5" t="s">
@@ -6729,7 +6815,7 @@
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="2" t="s">
+      <c r="A280" s="3" t="s">
         <v>419</v>
       </c>
       <c r="B280" s="1" t="s">
@@ -9804,7 +9890,7 @@
       </c>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A469" s="1" t="s">
+      <c r="A469" s="2" t="s">
         <v>676</v>
       </c>
       <c r="B469" s="1" t="s">
@@ -9824,7 +9910,7 @@
       </c>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A470" s="1" t="s">
+      <c r="A470" s="2" t="s">
         <v>678</v>
       </c>
       <c r="B470" s="1" t="s">
@@ -9844,7 +9930,7 @@
       </c>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A471" s="1" t="s">
+      <c r="A471" s="2" t="s">
         <v>679</v>
       </c>
       <c r="B471" s="1" t="s">
@@ -9861,7 +9947,7 @@
       </c>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A472" s="1" t="s">
+      <c r="A472" s="2" t="s">
         <v>680</v>
       </c>
       <c r="B472" s="1" t="s">
@@ -9881,7 +9967,7 @@
       </c>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A473" s="1" t="s">
+      <c r="A473" s="2" t="s">
         <v>681</v>
       </c>
       <c r="B473" s="1" t="s">
@@ -9901,7 +9987,7 @@
       </c>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A474" s="1" t="s">
+      <c r="A474" s="2" t="s">
         <v>682</v>
       </c>
       <c r="B474" s="1" t="s">
@@ -9921,7 +10007,7 @@
       </c>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A475" s="1" t="s">
+      <c r="A475" s="2" t="s">
         <v>683</v>
       </c>
       <c r="B475" s="1" t="s">
@@ -9941,7 +10027,7 @@
       </c>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A476" s="1" t="s">
+      <c r="A476" s="2" t="s">
         <v>685</v>
       </c>
       <c r="B476" s="1" t="s">
@@ -9961,7 +10047,7 @@
       </c>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A477" s="1" t="s">
+      <c r="A477" s="2" t="s">
         <v>686</v>
       </c>
       <c r="B477" s="1" t="s">
@@ -9981,7 +10067,7 @@
       </c>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A478" s="1" t="s">
+      <c r="A478" s="2" t="s">
         <v>687</v>
       </c>
       <c r="B478" s="1" t="s">
@@ -10001,7 +10087,7 @@
       </c>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A479" s="1" t="s">
+      <c r="A479" s="2" t="s">
         <v>688</v>
       </c>
       <c r="B479" s="1" t="s">
@@ -10012,7 +10098,7 @@
       </c>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A480" s="1" t="s">
+      <c r="A480" s="2" t="s">
         <v>689</v>
       </c>
       <c r="B480" s="1" t="s">
@@ -10023,7 +10109,7 @@
       </c>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A481" s="1" t="s">
+      <c r="A481" s="2" t="s">
         <v>690</v>
       </c>
       <c r="B481" s="1" t="s">
@@ -10034,7 +10120,7 @@
       </c>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="1" t="s">
+      <c r="A482" s="2" t="s">
         <v>691</v>
       </c>
       <c r="B482" s="1" t="s">
@@ -10045,7 +10131,7 @@
       </c>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A483" s="1" t="s">
+      <c r="A483" s="2" t="s">
         <v>692</v>
       </c>
       <c r="B483" s="1" t="s">
@@ -10056,7 +10142,7 @@
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A484" s="1" t="s">
+      <c r="A484" s="2" t="s">
         <v>694</v>
       </c>
       <c r="B484" s="1" t="s">
@@ -10067,7 +10153,7 @@
       </c>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A485" s="1" t="s">
+      <c r="A485" s="2" t="s">
         <v>696</v>
       </c>
       <c r="B485" s="1" t="s">
@@ -10087,7 +10173,7 @@
       </c>
     </row>
     <row r="486" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A486" s="1" t="s">
+      <c r="A486" s="2" t="s">
         <v>697</v>
       </c>
       <c r="B486" s="1" t="s">
@@ -10098,7 +10184,7 @@
       </c>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A487" s="1" t="s">
+      <c r="A487" s="2" t="s">
         <v>699</v>
       </c>
       <c r="B487" s="1" t="s">
@@ -10109,7 +10195,7 @@
       </c>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A488" s="1" t="s">
+      <c r="A488" s="2" t="s">
         <v>701</v>
       </c>
       <c r="B488" s="1" t="s">
@@ -10120,7 +10206,7 @@
       </c>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A489" s="1" t="s">
+      <c r="A489" s="2" t="s">
         <v>703</v>
       </c>
       <c r="B489" s="1" t="s">
@@ -10140,7 +10226,7 @@
       </c>
     </row>
     <row r="490" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A490" s="1" t="s">
+      <c r="A490" s="2" t="s">
         <v>704</v>
       </c>
       <c r="B490" s="1" t="s">
@@ -10151,7 +10237,7 @@
       </c>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A491" s="1" t="s">
+      <c r="A491" s="2" t="s">
         <v>705</v>
       </c>
       <c r="B491" s="1" t="s">
@@ -10171,7 +10257,7 @@
       </c>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A492" s="1" t="s">
+      <c r="A492" s="2" t="s">
         <v>706</v>
       </c>
       <c r="B492" s="1" t="s">
@@ -10182,7 +10268,7 @@
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A493" s="1" t="s">
+      <c r="A493" s="2" t="s">
         <v>707</v>
       </c>
       <c r="B493" s="1" t="s">
@@ -10202,7 +10288,7 @@
       </c>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A494" s="1" t="s">
+      <c r="A494" s="2" t="s">
         <v>709</v>
       </c>
       <c r="B494" s="1" t="s">
@@ -10213,7 +10299,7 @@
       </c>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A495" s="1" t="s">
+      <c r="A495" s="2" t="s">
         <v>710</v>
       </c>
       <c r="B495" s="1" t="s">
@@ -10236,8 +10322,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>